<commit_message>
update final M_C file with merged df
</commit_message>
<xml_diff>
--- a/crimecode_descriptions_by color.xlsx
+++ b/crimecode_descriptions_by color.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chr\Documents\Bootcamp\project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD84016D-DC8D-4D31-A1A6-8D1DDB847270}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFB75A3-64FF-4237-A34B-A6E25D55734D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="172">
   <si>
     <t>BATTERY - SIMPLE ASSAULT</t>
   </si>
@@ -491,9 +491,6 @@
   </si>
   <si>
     <t>OTHER NON-VIOLENT CRIMES</t>
-  </si>
-  <si>
-    <t>Combined Categories</t>
   </si>
   <si>
     <t>Original Crime Description</t>
@@ -568,6 +565,9 @@
   </si>
   <si>
     <t>THEFT / ATTEMPTED THEFT</t>
+  </si>
+  <si>
+    <t>New Combined Categories</t>
   </si>
 </sst>
 </file>
@@ -1557,7 +1557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1571,27 +1573,27 @@
   <sheetData>
     <row r="1" spans="1:8" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>158</v>
-      </c>
       <c r="G1" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>166</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>149</v>
@@ -1605,10 +1607,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -1619,10 +1621,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>2</v>
@@ -1636,10 +1638,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -1650,10 +1652,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>4</v>
@@ -1662,12 +1664,12 @@
         <v>133129</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>154</v>
@@ -1681,7 +1683,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>149</v>
@@ -1695,7 +1697,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>153</v>
@@ -1709,7 +1711,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>153</v>
@@ -1723,7 +1725,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>152</v>
@@ -1737,10 +1739,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>10</v>
@@ -1749,15 +1751,15 @@
         <v>77444</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -1768,10 +1770,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>12</v>
@@ -1785,7 +1787,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>155</v>
@@ -1799,10 +1801,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>14</v>
@@ -1811,15 +1813,15 @@
         <v>42225</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>15</v>
@@ -1833,7 +1835,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>155</v>
@@ -1847,7 +1849,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>155</v>
@@ -1859,12 +1861,12 @@
         <v>18847</v>
       </c>
       <c r="E19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>155</v>
@@ -1878,7 +1880,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>155</v>
@@ -1892,7 +1894,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>155</v>
@@ -1906,7 +1908,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>155</v>
@@ -1920,10 +1922,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>22</v>
@@ -1933,15 +1935,15 @@
       </c>
       <c r="E24" s="9"/>
       <c r="G24" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>23</v>
@@ -1953,7 +1955,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>152</v>
@@ -1967,10 +1969,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>25</v>
@@ -1979,15 +1981,15 @@
         <v>11744</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>26</v>
@@ -1998,10 +2000,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -2012,10 +2014,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>28</v>
@@ -2026,10 +2028,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>29</v>
@@ -2040,7 +2042,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>149</v>
@@ -2054,7 +2056,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>153</v>
@@ -2068,10 +2070,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>32</v>
@@ -2085,10 +2087,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>33</v>
@@ -2102,10 +2104,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>34</v>
@@ -2116,10 +2118,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>35</v>
@@ -2133,10 +2135,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>36</v>
@@ -2147,10 +2149,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>37</v>
@@ -2159,15 +2161,15 @@
         <v>4714</v>
       </c>
       <c r="E39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>38</v>
@@ -2176,12 +2178,12 @@
         <v>4302</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>149</v>
@@ -2195,10 +2197,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>40</v>
@@ -2212,7 +2214,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>155</v>
@@ -2226,10 +2228,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>42</v>
@@ -2240,10 +2242,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>43</v>
@@ -2254,7 +2256,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>155</v>
@@ -2268,10 +2270,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>45</v>
@@ -2282,7 +2284,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>155</v>
@@ -2296,10 +2298,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>47</v>
@@ -2308,12 +2310,12 @@
         <v>3000</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>149</v>
@@ -2327,7 +2329,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>155</v>
@@ -2341,7 +2343,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>155</v>
@@ -2355,7 +2357,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>155</v>
@@ -2369,10 +2371,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>52</v>
@@ -2383,7 +2385,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>150</v>
@@ -2397,10 +2399,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>54</v>
@@ -2411,7 +2413,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>155</v>
@@ -2425,10 +2427,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>56</v>
@@ -2437,15 +2439,15 @@
         <v>1959</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>57</v>
@@ -2456,10 +2458,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>58</v>
@@ -2468,15 +2470,15 @@
         <v>1698</v>
       </c>
       <c r="E60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>59</v>
@@ -2487,10 +2489,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>60</v>
@@ -2499,12 +2501,12 @@
         <v>1520</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>152</v>
@@ -2518,7 +2520,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>152</v>
@@ -2532,10 +2534,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>63</v>
@@ -2546,10 +2548,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>64</v>
@@ -2560,7 +2562,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>155</v>
@@ -2574,7 +2576,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>155</v>
@@ -2588,10 +2590,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>67</v>
@@ -2600,12 +2602,12 @@
         <v>1239</v>
       </c>
       <c r="E69" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>155</v>
@@ -2619,10 +2621,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>69</v>
@@ -2631,15 +2633,15 @@
         <v>1105</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>70</v>
@@ -2648,15 +2650,15 @@
         <v>1096</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>71</v>
@@ -2667,7 +2669,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B74" s="12" t="s">
         <v>155</v>
@@ -2681,10 +2683,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>73</v>
@@ -2695,10 +2697,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>74</v>
@@ -2707,15 +2709,15 @@
         <v>1020</v>
       </c>
       <c r="E76" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>75</v>
@@ -2726,10 +2728,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>76</v>
@@ -2738,12 +2740,12 @@
         <v>872</v>
       </c>
       <c r="E78" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>155</v>
@@ -2757,10 +2759,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>78</v>
@@ -2769,15 +2771,15 @@
         <v>785</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>79</v>
@@ -2788,7 +2790,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B82" s="12" t="s">
         <v>155</v>
@@ -2802,10 +2804,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>81</v>
@@ -2816,10 +2818,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>82</v>
@@ -2833,10 +2835,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>83</v>
@@ -2847,10 +2849,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>84</v>
@@ -2859,15 +2861,15 @@
         <v>612</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C87" s="11" t="s">
         <v>85</v>
@@ -2876,12 +2878,12 @@
         <v>539</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B88" s="12" t="s">
         <v>155</v>
@@ -2895,7 +2897,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B89" s="12" t="s">
         <v>155</v>
@@ -2909,7 +2911,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B90" s="12" t="s">
         <v>155</v>
@@ -2923,7 +2925,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B91" s="12" t="s">
         <v>155</v>
@@ -2937,7 +2939,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B92" s="12" t="s">
         <v>155</v>
@@ -2951,7 +2953,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>155</v>
@@ -2965,10 +2967,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>92</v>
@@ -2979,7 +2981,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>149</v>
@@ -2993,10 +2995,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>94</v>
@@ -3007,7 +3009,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>155</v>
@@ -3021,10 +3023,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>96</v>
@@ -3033,15 +3035,15 @@
         <v>262</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C99" s="11" t="s">
         <v>97</v>
@@ -3055,10 +3057,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C100" s="11" t="s">
         <v>98</v>
@@ -3067,15 +3069,15 @@
         <v>244</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C101" s="13" t="s">
         <v>99</v>
@@ -3086,7 +3088,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B102" s="12" t="s">
         <v>155</v>
@@ -3100,10 +3102,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C103" s="11" t="s">
         <v>101</v>
@@ -3112,15 +3114,15 @@
         <v>213</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C104" s="11" t="s">
         <v>102</v>
@@ -3129,15 +3131,15 @@
         <v>205</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C105" s="11" t="s">
         <v>103</v>
@@ -3146,15 +3148,15 @@
         <v>192</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>104</v>
@@ -3165,7 +3167,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B107" s="12" t="s">
         <v>155</v>
@@ -3179,10 +3181,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C108" s="13" t="s">
         <v>106</v>
@@ -3193,10 +3195,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C109" s="11" t="s">
         <v>107</v>
@@ -3210,10 +3212,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>108</v>
@@ -3224,10 +3226,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C111" s="11" t="s">
         <v>109</v>
@@ -3236,15 +3238,15 @@
         <v>115</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>110</v>
@@ -3255,10 +3257,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>111</v>
@@ -3269,10 +3271,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C114" s="11" t="s">
         <v>112</v>
@@ -3281,15 +3283,15 @@
         <v>88</v>
       </c>
       <c r="G114" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C115" s="14" t="s">
         <v>113</v>
@@ -3300,10 +3302,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C116" s="11" t="s">
         <v>114</v>
@@ -3317,7 +3319,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B117" s="12" t="s">
         <v>155</v>
@@ -3331,7 +3333,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B118" s="12" t="s">
         <v>155</v>
@@ -3345,10 +3347,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C119" s="11" t="s">
         <v>117</v>
@@ -3357,15 +3359,15 @@
         <v>44</v>
       </c>
       <c r="G119" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C120" s="13" t="s">
         <v>118</v>
@@ -3376,7 +3378,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B121" s="12" t="s">
         <v>155</v>
@@ -3390,10 +3392,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C122" s="11" t="s">
         <v>120</v>
@@ -3407,7 +3409,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B123" s="12" t="s">
         <v>155</v>
@@ -3421,7 +3423,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B124" s="12" t="s">
         <v>155</v>
@@ -3435,10 +3437,10 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C125" s="11" t="s">
         <v>123</v>
@@ -3447,15 +3449,15 @@
         <v>34</v>
       </c>
       <c r="G125" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>124</v>
@@ -3466,7 +3468,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B127" s="12" t="s">
         <v>155</v>
@@ -3480,7 +3482,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B128" s="12" t="s">
         <v>155</v>
@@ -3494,10 +3496,10 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C129" s="11" t="s">
         <v>127</v>
@@ -3506,15 +3508,15 @@
         <v>23</v>
       </c>
       <c r="G129" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>128</v>
@@ -3525,10 +3527,10 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>129</v>
@@ -3539,10 +3541,10 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C132" s="11" t="s">
         <v>130</v>
@@ -3551,12 +3553,12 @@
         <v>21</v>
       </c>
       <c r="G132" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B133" s="12" t="s">
         <v>155</v>
@@ -3570,10 +3572,10 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C134" s="11" t="s">
         <v>132</v>
@@ -3582,12 +3584,12 @@
         <v>20</v>
       </c>
       <c r="G134" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B135" s="12" t="s">
         <v>155</v>
@@ -3601,10 +3603,10 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C136" s="11" t="s">
         <v>134</v>
@@ -3618,7 +3620,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B137" s="12" t="s">
         <v>155</v>
@@ -3632,10 +3634,10 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C138" s="11" t="s">
         <v>136</v>
@@ -3649,7 +3651,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B139" s="12" t="s">
         <v>155</v>
@@ -3663,10 +3665,10 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>138</v>
@@ -3677,10 +3679,10 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C141" s="11" t="s">
         <v>139</v>
@@ -3689,12 +3691,12 @@
         <v>8</v>
       </c>
       <c r="G141" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B142" s="12" t="s">
         <v>155</v>
@@ -3708,10 +3710,10 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C143" s="13" t="s">
         <v>141</v>
@@ -3722,7 +3724,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B144" s="12" t="s">
         <v>155</v>
@@ -3736,7 +3738,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B145" s="12" t="s">
         <v>155</v>
@@ -3750,7 +3752,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B146" s="12" t="s">
         <v>155</v>
@@ -3764,7 +3766,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B147" s="12" t="s">
         <v>155</v>
@@ -3778,7 +3780,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B148" s="12" t="s">
         <v>155</v>
@@ -3792,7 +3794,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B149" s="12" t="s">
         <v>155</v>
@@ -3806,10 +3808,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>148</v>

</xml_diff>